<commit_message>
sample data was missing bioproject ID
</commit_message>
<xml_diff>
--- a/assets/sample_metadata/mpxv_user_provided_annotations_metadata.xlsx
+++ b/assets/sample_metadata/mpxv_user_provided_annotations_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\sample_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DE84F7-9239-4752-BB40-D4A7EAE4B22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FBE7CB-EBE1-495E-A413-3D2803EB3321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="455">
   <si>
     <t>Strategy</t>
   </si>
@@ -1397,6 +1397,12 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>test_group</t>
+  </si>
+  <si>
+    <t>PRJNA849962</t>
   </si>
 </sst>
 </file>
@@ -2112,10 +2118,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BB45"/>
+  <dimension ref="A1:BA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2128,22 +2134,22 @@
     <col min="8" max="12" width="15.1796875" customWidth="1"/>
     <col min="13" max="13" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.453125" customWidth="1"/>
-    <col min="16" max="17" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="31" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.453125" style="17" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="13.453125" style="17" customWidth="1"/>
-    <col min="35" max="35" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="36" max="41" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.453125" customWidth="1"/>
-    <col min="43" max="51" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="52" max="54" width="13.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="13.453125" style="17" customWidth="1"/>
+    <col min="34" max="34" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="40" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.453125" customWidth="1"/>
+    <col min="42" max="50" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="13.453125" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="18.75" customHeight="1">
+    <row r="1" spans="1:53" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>317</v>
       </c>
@@ -2152,23 +2158,23 @@
         <v>318</v>
       </c>
       <c r="N1" s="46"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Y1" s="36" t="s">
         <v>319</v>
       </c>
-      <c r="AD1" s="36" t="s">
+      <c r="AC1" s="36" t="s">
         <v>320</v>
       </c>
+      <c r="AH1" s="36" t="s">
+        <v>321</v>
+      </c>
       <c r="AI1" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="AJ1" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="AS1" s="36" t="s">
+      <c r="AR1" s="36" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="18.75" customHeight="1">
+    <row r="2" spans="1:53" ht="18.75" customHeight="1">
       <c r="A2" s="45" t="s">
         <v>440</v>
       </c>
@@ -2211,131 +2217,137 @@
       <c r="N2" s="47" t="s">
         <v>415</v>
       </c>
+      <c r="O2" s="20" t="s">
+        <v>369</v>
+      </c>
       <c r="P2" s="20" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="R2" s="20" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="S2" s="20" t="s">
-        <v>372</v>
+        <v>287</v>
       </c>
       <c r="T2" s="20" t="s">
-        <v>287</v>
+        <v>233</v>
       </c>
       <c r="U2" s="20" t="s">
-        <v>233</v>
+        <v>324</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="W2" s="20" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
       <c r="X2" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="Y2" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Y2" s="37" t="s">
         <v>231</v>
       </c>
+      <c r="Z2" s="20" t="s">
+        <v>232</v>
+      </c>
       <c r="AA2" s="20" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="AB2" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="AC2" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="AD2" s="37" t="s">
+      <c r="AC2" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="AF2" s="21" t="s">
+      <c r="AE2" s="21" t="s">
         <v>242</v>
       </c>
+      <c r="AF2" s="48" t="s">
+        <v>421</v>
+      </c>
       <c r="AG2" s="48" t="s">
-        <v>421</v>
-      </c>
-      <c r="AH2" s="48" t="s">
         <v>443</v>
       </c>
+      <c r="AH2" s="37" t="s">
+        <v>224</v>
+      </c>
       <c r="AI2" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="AJ2" s="37" t="s">
         <v>288</v>
       </c>
+      <c r="AJ2" s="20" t="s">
+        <v>326</v>
+      </c>
       <c r="AK2" s="20" t="s">
-        <v>326</v>
+        <v>290</v>
       </c>
       <c r="AL2" s="20" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AM2" s="20" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AN2" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="AO2" s="20" t="s">
         <v>327</v>
       </c>
+      <c r="AO2" s="45" t="s">
+        <v>413</v>
+      </c>
       <c r="AP2" s="45" t="s">
-        <v>413</v>
-      </c>
-      <c r="AQ2" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="AR2" s="20" t="s">
+      <c r="AQ2" s="20" t="s">
         <v>299</v>
       </c>
-      <c r="AS2" s="37" t="s">
+      <c r="AR2" s="37" t="s">
         <v>293</v>
       </c>
+      <c r="AS2" s="20" t="s">
+        <v>328</v>
+      </c>
       <c r="AT2" s="20" t="s">
-        <v>328</v>
+        <v>295</v>
       </c>
       <c r="AU2" s="20" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AV2" s="20" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="AW2" s="20" t="s">
-        <v>297</v>
+        <v>329</v>
       </c>
       <c r="AX2" s="20" t="s">
-        <v>329</v>
-      </c>
-      <c r="AY2" s="20" t="s">
         <v>300</v>
       </c>
+      <c r="AY2" s="21" t="s">
+        <v>373</v>
+      </c>
       <c r="AZ2" s="21" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="BA2" s="21" t="s">
-        <v>374</v>
-      </c>
-      <c r="BB2" s="21" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:54" ht="18.75" customHeight="1">
+    <row r="3" spans="1:53" ht="18.75" customHeight="1">
       <c r="A3" t="s">
         <v>384</v>
       </c>
       <c r="B3" t="s">
         <v>385</v>
       </c>
+      <c r="C3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D3" t="s">
+        <v>454</v>
+      </c>
       <c r="E3" t="s">
         <v>450</v>
       </c>
@@ -2348,82 +2360,88 @@
       <c r="M3" t="s">
         <v>385</v>
       </c>
+      <c r="P3" t="s">
+        <v>257</v>
+      </c>
       <c r="Q3" t="s">
-        <v>257</v>
+        <v>378</v>
       </c>
       <c r="R3" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="S3" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="T3" t="s">
-        <v>307</v>
-      </c>
-      <c r="U3" t="s">
         <v>387</v>
       </c>
-      <c r="X3" t="s">
+      <c r="W3" t="s">
         <v>388</v>
       </c>
-      <c r="Z3" s="36"/>
-      <c r="AD3" t="s">
+      <c r="Y3" s="36"/>
+      <c r="AC3" t="s">
         <v>389</v>
       </c>
-      <c r="AF3" s="14">
+      <c r="AE3" s="14">
         <v>40</v>
       </c>
+      <c r="AF3" s="14" t="s">
+        <v>423</v>
+      </c>
       <c r="AG3" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="AH3" s="14" t="s">
         <v>444</v>
       </c>
+      <c r="AH3" t="s">
+        <v>390</v>
+      </c>
       <c r="AI3" t="s">
-        <v>390</v>
+        <v>216</v>
       </c>
       <c r="AJ3" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="AK3" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="AL3" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="AM3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN3" t="s">
         <v>310</v>
       </c>
+      <c r="AO3" t="s">
+        <v>414</v>
+      </c>
       <c r="AP3" t="s">
-        <v>414</v>
+        <v>428</v>
       </c>
       <c r="AQ3" t="s">
-        <v>428</v>
-      </c>
-      <c r="AR3" t="s">
         <v>433</v>
       </c>
-      <c r="AS3" s="36"/>
-      <c r="AZ3" s="14">
+      <c r="AR3" s="36"/>
+      <c r="AY3" s="14">
         <v>5</v>
       </c>
-      <c r="BA3" s="50" t="s">
+      <c r="AZ3" s="50" t="s">
         <v>437</v>
       </c>
-      <c r="BB3" s="14">
+      <c r="BA3" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:54" ht="18.75" customHeight="1">
+    <row r="4" spans="1:53" ht="18.75" customHeight="1">
       <c r="A4" t="s">
         <v>391</v>
       </c>
       <c r="B4" t="s">
         <v>392</v>
       </c>
+      <c r="C4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" t="s">
+        <v>454</v>
+      </c>
       <c r="E4" t="s">
         <v>450</v>
       </c>
@@ -2436,82 +2454,88 @@
       <c r="M4" t="s">
         <v>392</v>
       </c>
+      <c r="P4" t="s">
+        <v>257</v>
+      </c>
       <c r="Q4" t="s">
-        <v>257</v>
+        <v>378</v>
       </c>
       <c r="R4" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="S4" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="T4" t="s">
-        <v>307</v>
-      </c>
-      <c r="U4" t="s">
         <v>394</v>
       </c>
-      <c r="X4" t="s">
+      <c r="W4" t="s">
         <v>395</v>
       </c>
-      <c r="Z4" s="36"/>
-      <c r="AD4" t="s">
+      <c r="Y4" s="36"/>
+      <c r="AC4" t="s">
         <v>396</v>
       </c>
-      <c r="AF4" s="14">
+      <c r="AE4" s="14">
         <v>121</v>
       </c>
+      <c r="AF4" s="14" t="s">
+        <v>424</v>
+      </c>
       <c r="AG4" s="14" t="s">
-        <v>424</v>
-      </c>
-      <c r="AH4" s="14" t="s">
         <v>445</v>
       </c>
+      <c r="AH4" t="s">
+        <v>397</v>
+      </c>
       <c r="AI4" t="s">
-        <v>397</v>
+        <v>216</v>
       </c>
       <c r="AJ4" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="AK4" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="AL4" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="AM4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN4" t="s">
         <v>310</v>
       </c>
+      <c r="AO4" t="s">
+        <v>414</v>
+      </c>
       <c r="AP4" t="s">
-        <v>414</v>
+        <v>429</v>
       </c>
       <c r="AQ4" t="s">
-        <v>429</v>
-      </c>
-      <c r="AR4" t="s">
         <v>434</v>
       </c>
-      <c r="AS4" s="36"/>
-      <c r="AZ4" s="14">
+      <c r="AR4" s="36"/>
+      <c r="AY4" s="14">
         <v>8</v>
       </c>
-      <c r="BA4" s="49" t="s">
+      <c r="AZ4" s="49" t="s">
         <v>438</v>
       </c>
-      <c r="BB4" s="14">
+      <c r="BA4" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:54" ht="18.75" customHeight="1">
+    <row r="5" spans="1:53" ht="18.75" customHeight="1">
       <c r="A5" t="s">
         <v>398</v>
       </c>
       <c r="B5" t="s">
         <v>399</v>
       </c>
+      <c r="C5" t="s">
+        <v>453</v>
+      </c>
+      <c r="D5" t="s">
+        <v>454</v>
+      </c>
       <c r="E5" t="s">
         <v>450</v>
       </c>
@@ -2524,85 +2548,91 @@
       <c r="M5" t="s">
         <v>399</v>
       </c>
+      <c r="P5" t="s">
+        <v>257</v>
+      </c>
       <c r="Q5" t="s">
-        <v>257</v>
+        <v>378</v>
       </c>
       <c r="R5" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="S5" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="T5" t="s">
-        <v>307</v>
+        <v>394</v>
       </c>
       <c r="U5" t="s">
-        <v>394</v>
-      </c>
-      <c r="V5" t="s">
         <v>379</v>
       </c>
-      <c r="X5" t="s">
+      <c r="W5" t="s">
         <v>400</v>
       </c>
-      <c r="Z5" s="36"/>
-      <c r="AD5" t="s">
+      <c r="Y5" s="36"/>
+      <c r="AC5" t="s">
         <v>401</v>
       </c>
-      <c r="AF5" s="14">
+      <c r="AE5" s="14">
         <v>72</v>
       </c>
+      <c r="AF5" s="14" t="s">
+        <v>425</v>
+      </c>
       <c r="AG5" s="14" t="s">
-        <v>425</v>
-      </c>
-      <c r="AH5" s="14" t="s">
         <v>446</v>
       </c>
+      <c r="AH5" t="s">
+        <v>402</v>
+      </c>
       <c r="AI5" t="s">
-        <v>402</v>
+        <v>216</v>
       </c>
       <c r="AJ5" t="s">
-        <v>216</v>
+        <v>4</v>
       </c>
       <c r="AK5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>310</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>414</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>430</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>435</v>
+      </c>
+      <c r="AR5" s="36"/>
+      <c r="AY5" s="14">
         <v>4</v>
       </c>
-      <c r="AL5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>310</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>414</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>430</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>435</v>
-      </c>
-      <c r="AS5" s="36"/>
-      <c r="AZ5" s="14">
-        <v>4</v>
-      </c>
-      <c r="BA5" s="50" t="s">
+      <c r="AZ5" s="50" t="s">
         <v>439</v>
       </c>
-      <c r="BB5" s="14">
+      <c r="BA5" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:54" ht="18.75" customHeight="1">
+    <row r="6" spans="1:53" ht="18.75" customHeight="1">
       <c r="A6" t="s">
         <v>441</v>
       </c>
       <c r="B6" t="s">
         <v>403</v>
       </c>
+      <c r="C6" t="s">
+        <v>453</v>
+      </c>
+      <c r="D6" t="s">
+        <v>454</v>
+      </c>
       <c r="E6" t="s">
         <v>450</v>
       </c>
@@ -2615,85 +2645,91 @@
       <c r="M6" t="s">
         <v>403</v>
       </c>
+      <c r="P6" t="s">
+        <v>257</v>
+      </c>
       <c r="Q6" t="s">
-        <v>257</v>
+        <v>378</v>
       </c>
       <c r="R6" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="S6" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="T6" t="s">
-        <v>307</v>
+        <v>405</v>
       </c>
       <c r="U6" t="s">
+        <v>379</v>
+      </c>
+      <c r="W6" t="s">
+        <v>380</v>
+      </c>
+      <c r="Y6" s="36"/>
+      <c r="AC6" t="s">
+        <v>406</v>
+      </c>
+      <c r="AE6" s="14">
+        <v>73</v>
+      </c>
+      <c r="AF6" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="AG6" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>407</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>310</v>
+      </c>
+      <c r="AO6" t="s">
+        <v>414</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>431</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>436</v>
+      </c>
+      <c r="AR6" s="36"/>
+      <c r="AY6" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="AZ6" s="50" t="s">
         <v>405</v>
       </c>
-      <c r="V6" t="s">
-        <v>379</v>
-      </c>
-      <c r="X6" t="s">
-        <v>380</v>
-      </c>
-      <c r="Z6" s="36"/>
-      <c r="AD6" t="s">
-        <v>406</v>
-      </c>
-      <c r="AF6" s="14">
-        <v>73</v>
-      </c>
-      <c r="AG6" s="14" t="s">
-        <v>426</v>
-      </c>
-      <c r="AH6" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>407</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>216</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>310</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>414</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>431</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>436</v>
-      </c>
-      <c r="AS6" s="36"/>
-      <c r="AZ6" s="17" t="s">
-        <v>408</v>
-      </c>
-      <c r="BA6" s="50" t="s">
-        <v>405</v>
-      </c>
-      <c r="BB6" s="14">
+      <c r="BA6" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:54" ht="18.75" customHeight="1">
+    <row r="7" spans="1:53" ht="18.75" customHeight="1">
       <c r="A7" t="s">
         <v>442</v>
       </c>
       <c r="B7" t="s">
         <v>376</v>
       </c>
+      <c r="C7" t="s">
+        <v>453</v>
+      </c>
+      <c r="D7" t="s">
+        <v>454</v>
+      </c>
       <c r="E7" t="s">
         <v>450</v>
       </c>
@@ -2706,454 +2742,454 @@
       <c r="M7" t="s">
         <v>376</v>
       </c>
+      <c r="P7" t="s">
+        <v>257</v>
+      </c>
       <c r="Q7" t="s">
-        <v>257</v>
+        <v>378</v>
       </c>
       <c r="R7" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
       <c r="S7" t="s">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="T7" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="U7" t="s">
+        <v>379</v>
+      </c>
+      <c r="W7" t="s">
+        <v>380</v>
+      </c>
+      <c r="Y7" s="36"/>
+      <c r="AC7" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE7" s="14">
+        <v>247</v>
+      </c>
+      <c r="AF7" s="49" t="s">
+        <v>422</v>
+      </c>
+      <c r="AG7" s="49" t="s">
+        <v>448</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>382</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>216</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>310</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>414</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>427</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>432</v>
+      </c>
+      <c r="AR7" s="36"/>
+      <c r="AY7" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="AZ7" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="V7" t="s">
-        <v>379</v>
-      </c>
-      <c r="X7" t="s">
-        <v>380</v>
-      </c>
-      <c r="Z7" s="36"/>
-      <c r="AD7" t="s">
-        <v>381</v>
-      </c>
-      <c r="AF7" s="14">
-        <v>247</v>
-      </c>
-      <c r="AG7" s="49" t="s">
-        <v>422</v>
-      </c>
-      <c r="AH7" s="49" t="s">
-        <v>448</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>382</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>216</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>310</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>414</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>427</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>432</v>
-      </c>
-      <c r="AS7" s="36"/>
-      <c r="AZ7" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="BA7" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="BB7" s="14">
+      <c r="BA7" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:54" ht="18.75" customHeight="1">
-      <c r="Z8" s="36"/>
+    <row r="8" spans="1:53" ht="18.75" customHeight="1">
+      <c r="Y8" s="36"/>
+      <c r="AE8" s="14"/>
       <c r="AF8" s="14"/>
       <c r="AG8" s="14"/>
-      <c r="AH8" s="14"/>
-      <c r="AS8" s="36"/>
-    </row>
-    <row r="9" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR8" s="36"/>
+    </row>
+    <row r="9" spans="1:53" ht="18.75" customHeight="1">
       <c r="F9" s="46"/>
       <c r="M9" s="36"/>
       <c r="N9" s="46"/>
-      <c r="Z9" s="36"/>
-      <c r="AD9" s="36"/>
+      <c r="Y9" s="36"/>
+      <c r="AC9" s="36"/>
+      <c r="AH9" s="36"/>
       <c r="AI9" s="36"/>
-      <c r="AJ9" s="36"/>
-      <c r="AS9" s="36"/>
-    </row>
-    <row r="10" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR9" s="36"/>
+    </row>
+    <row r="10" spans="1:53" ht="18.75" customHeight="1">
       <c r="F10" s="46"/>
       <c r="M10" s="36"/>
       <c r="N10" s="46"/>
-      <c r="Z10" s="36"/>
-      <c r="AD10" s="36"/>
+      <c r="Y10" s="36"/>
+      <c r="AC10" s="36"/>
+      <c r="AH10" s="36"/>
       <c r="AI10" s="36"/>
-      <c r="AJ10" s="36"/>
-      <c r="AS10" s="36"/>
-    </row>
-    <row r="11" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR10" s="36"/>
+    </row>
+    <row r="11" spans="1:53" ht="18.75" customHeight="1">
       <c r="F11" s="46"/>
       <c r="M11" s="36"/>
       <c r="N11" s="46"/>
-      <c r="Z11" s="36"/>
-      <c r="AD11" s="36"/>
+      <c r="Y11" s="36"/>
+      <c r="AC11" s="36"/>
+      <c r="AH11" s="36"/>
       <c r="AI11" s="36"/>
-      <c r="AJ11" s="36"/>
-      <c r="AS11" s="36"/>
-    </row>
-    <row r="12" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR11" s="36"/>
+    </row>
+    <row r="12" spans="1:53" ht="18.75" customHeight="1">
       <c r="F12" s="46"/>
       <c r="M12" s="36"/>
       <c r="N12" s="46"/>
-      <c r="Z12" s="36"/>
-      <c r="AD12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="AC12" s="36"/>
+      <c r="AH12" s="36"/>
       <c r="AI12" s="36"/>
-      <c r="AJ12" s="36"/>
-      <c r="AS12" s="36"/>
-    </row>
-    <row r="13" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR12" s="36"/>
+    </row>
+    <row r="13" spans="1:53" ht="18.75" customHeight="1">
       <c r="F13" s="46"/>
       <c r="M13" s="36"/>
       <c r="N13" s="46"/>
-      <c r="Z13" s="36"/>
-      <c r="AD13" s="36"/>
+      <c r="Y13" s="36"/>
+      <c r="AC13" s="36"/>
+      <c r="AH13" s="36"/>
       <c r="AI13" s="36"/>
-      <c r="AJ13" s="36"/>
-      <c r="AS13" s="36"/>
-    </row>
-    <row r="14" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR13" s="36"/>
+    </row>
+    <row r="14" spans="1:53" ht="18.75" customHeight="1">
       <c r="F14" s="46"/>
       <c r="M14" s="36"/>
       <c r="N14" s="46"/>
-      <c r="Z14" s="36"/>
-      <c r="AD14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="AC14" s="36"/>
+      <c r="AH14" s="36"/>
       <c r="AI14" s="36"/>
-      <c r="AJ14" s="36"/>
-      <c r="AS14" s="36"/>
-    </row>
-    <row r="15" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR14" s="36"/>
+    </row>
+    <row r="15" spans="1:53" ht="18.75" customHeight="1">
       <c r="F15" s="46"/>
       <c r="M15" s="36"/>
       <c r="N15" s="46"/>
-      <c r="Z15" s="36"/>
-      <c r="AD15" s="36"/>
+      <c r="Y15" s="36"/>
+      <c r="AC15" s="36"/>
+      <c r="AH15" s="36"/>
       <c r="AI15" s="36"/>
-      <c r="AJ15" s="36"/>
-      <c r="AS15" s="36"/>
-    </row>
-    <row r="16" spans="1:54" ht="18.75" customHeight="1">
+      <c r="AR15" s="36"/>
+    </row>
+    <row r="16" spans="1:53" ht="18.75" customHeight="1">
       <c r="F16" s="46"/>
       <c r="M16" s="36"/>
       <c r="N16" s="46"/>
-      <c r="Z16" s="36"/>
-      <c r="AD16" s="36"/>
+      <c r="Y16" s="36"/>
+      <c r="AC16" s="36"/>
+      <c r="AH16" s="36"/>
       <c r="AI16" s="36"/>
-      <c r="AJ16" s="36"/>
-      <c r="AS16" s="36"/>
-    </row>
-    <row r="17" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR16" s="36"/>
+    </row>
+    <row r="17" spans="6:44" ht="18.75" customHeight="1">
       <c r="F17" s="46"/>
       <c r="M17" s="36"/>
       <c r="N17" s="46"/>
-      <c r="Z17" s="36"/>
-      <c r="AD17" s="36"/>
+      <c r="Y17" s="36"/>
+      <c r="AC17" s="36"/>
+      <c r="AH17" s="36"/>
       <c r="AI17" s="36"/>
-      <c r="AJ17" s="36"/>
-      <c r="AS17" s="36"/>
-    </row>
-    <row r="18" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR17" s="36"/>
+    </row>
+    <row r="18" spans="6:44" ht="18.75" customHeight="1">
       <c r="F18" s="46"/>
       <c r="M18" s="36"/>
       <c r="N18" s="46"/>
-      <c r="Z18" s="36"/>
-      <c r="AD18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="AC18" s="36"/>
+      <c r="AH18" s="36"/>
       <c r="AI18" s="36"/>
-      <c r="AJ18" s="36"/>
-      <c r="AS18" s="36"/>
-    </row>
-    <row r="19" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR18" s="36"/>
+    </row>
+    <row r="19" spans="6:44" ht="18.75" customHeight="1">
       <c r="F19" s="46"/>
       <c r="M19" s="36"/>
       <c r="N19" s="46"/>
-      <c r="Z19" s="36"/>
-      <c r="AD19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AH19" s="36"/>
       <c r="AI19" s="36"/>
-      <c r="AJ19" s="36"/>
-      <c r="AS19" s="36"/>
-    </row>
-    <row r="20" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR19" s="36"/>
+    </row>
+    <row r="20" spans="6:44" ht="18.75" customHeight="1">
       <c r="F20" s="46"/>
       <c r="M20" s="36"/>
       <c r="N20" s="46"/>
-      <c r="Z20" s="36"/>
-      <c r="AD20" s="36"/>
+      <c r="Y20" s="36"/>
+      <c r="AC20" s="36"/>
+      <c r="AH20" s="36"/>
       <c r="AI20" s="36"/>
-      <c r="AJ20" s="36"/>
-      <c r="AS20" s="36"/>
-    </row>
-    <row r="21" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR20" s="36"/>
+    </row>
+    <row r="21" spans="6:44" ht="18.75" customHeight="1">
       <c r="F21" s="46"/>
       <c r="M21" s="36"/>
       <c r="N21" s="46"/>
-      <c r="Z21" s="36"/>
-      <c r="AD21" s="36"/>
+      <c r="Y21" s="36"/>
+      <c r="AC21" s="36"/>
+      <c r="AH21" s="36"/>
       <c r="AI21" s="36"/>
-      <c r="AJ21" s="36"/>
-      <c r="AS21" s="36"/>
-    </row>
-    <row r="22" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR21" s="36"/>
+    </row>
+    <row r="22" spans="6:44" ht="18.75" customHeight="1">
       <c r="F22" s="46"/>
       <c r="M22" s="36"/>
       <c r="N22" s="46"/>
-      <c r="Z22" s="36"/>
-      <c r="AD22" s="36"/>
+      <c r="Y22" s="36"/>
+      <c r="AC22" s="36"/>
+      <c r="AH22" s="36"/>
       <c r="AI22" s="36"/>
-      <c r="AJ22" s="36"/>
-      <c r="AS22" s="36"/>
-    </row>
-    <row r="23" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR22" s="36"/>
+    </row>
+    <row r="23" spans="6:44" ht="18.75" customHeight="1">
       <c r="F23" s="46"/>
       <c r="M23" s="36"/>
       <c r="N23" s="46"/>
-      <c r="Z23" s="36"/>
-      <c r="AD23" s="36"/>
+      <c r="Y23" s="36"/>
+      <c r="AC23" s="36"/>
+      <c r="AH23" s="36"/>
       <c r="AI23" s="36"/>
-      <c r="AJ23" s="36"/>
-      <c r="AS23" s="36"/>
-    </row>
-    <row r="24" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR23" s="36"/>
+    </row>
+    <row r="24" spans="6:44" ht="18.75" customHeight="1">
       <c r="F24" s="46"/>
       <c r="M24" s="36"/>
       <c r="N24" s="46"/>
-      <c r="Z24" s="36"/>
-      <c r="AD24" s="36"/>
+      <c r="Y24" s="36"/>
+      <c r="AC24" s="36"/>
+      <c r="AH24" s="36"/>
       <c r="AI24" s="36"/>
-      <c r="AJ24" s="36"/>
-      <c r="AS24" s="36"/>
-    </row>
-    <row r="25" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR24" s="36"/>
+    </row>
+    <row r="25" spans="6:44" ht="18.75" customHeight="1">
       <c r="F25" s="46"/>
       <c r="M25" s="36"/>
       <c r="N25" s="46"/>
-      <c r="Z25" s="36"/>
-      <c r="AD25" s="36"/>
+      <c r="Y25" s="36"/>
+      <c r="AC25" s="36"/>
+      <c r="AH25" s="36"/>
       <c r="AI25" s="36"/>
-      <c r="AJ25" s="36"/>
-      <c r="AS25" s="36"/>
-    </row>
-    <row r="26" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR25" s="36"/>
+    </row>
+    <row r="26" spans="6:44" ht="18.75" customHeight="1">
       <c r="F26" s="46"/>
       <c r="M26" s="36"/>
       <c r="N26" s="46"/>
-      <c r="Z26" s="36"/>
-      <c r="AD26" s="36"/>
+      <c r="Y26" s="36"/>
+      <c r="AC26" s="36"/>
+      <c r="AH26" s="36"/>
       <c r="AI26" s="36"/>
-      <c r="AJ26" s="36"/>
-      <c r="AS26" s="36"/>
-    </row>
-    <row r="27" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR26" s="36"/>
+    </row>
+    <row r="27" spans="6:44" ht="18.75" customHeight="1">
       <c r="F27" s="46"/>
       <c r="M27" s="36"/>
       <c r="N27" s="46"/>
-      <c r="Z27" s="36"/>
-      <c r="AD27" s="36"/>
+      <c r="Y27" s="36"/>
+      <c r="AC27" s="36"/>
+      <c r="AH27" s="36"/>
       <c r="AI27" s="36"/>
-      <c r="AJ27" s="36"/>
-      <c r="AS27" s="36"/>
-    </row>
-    <row r="28" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR27" s="36"/>
+    </row>
+    <row r="28" spans="6:44" ht="18.75" customHeight="1">
       <c r="F28" s="46"/>
       <c r="M28" s="36"/>
       <c r="N28" s="46"/>
-      <c r="Z28" s="36"/>
-      <c r="AD28" s="36"/>
+      <c r="Y28" s="36"/>
+      <c r="AC28" s="36"/>
+      <c r="AH28" s="36"/>
       <c r="AI28" s="36"/>
-      <c r="AJ28" s="36"/>
-      <c r="AS28" s="36"/>
-    </row>
-    <row r="29" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR28" s="36"/>
+    </row>
+    <row r="29" spans="6:44" ht="18.75" customHeight="1">
       <c r="F29" s="46"/>
       <c r="M29" s="36"/>
       <c r="N29" s="46"/>
-      <c r="Z29" s="36"/>
-      <c r="AD29" s="36"/>
+      <c r="Y29" s="36"/>
+      <c r="AC29" s="36"/>
+      <c r="AH29" s="36"/>
       <c r="AI29" s="36"/>
-      <c r="AJ29" s="36"/>
-      <c r="AS29" s="36"/>
-    </row>
-    <row r="30" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR29" s="36"/>
+    </row>
+    <row r="30" spans="6:44" ht="18.75" customHeight="1">
       <c r="F30" s="46"/>
       <c r="M30" s="36"/>
       <c r="N30" s="46"/>
-      <c r="Z30" s="36"/>
-      <c r="AD30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AH30" s="36"/>
       <c r="AI30" s="36"/>
-      <c r="AJ30" s="36"/>
-      <c r="AS30" s="36"/>
-    </row>
-    <row r="31" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR30" s="36"/>
+    </row>
+    <row r="31" spans="6:44" ht="18.75" customHeight="1">
       <c r="F31" s="46"/>
       <c r="M31" s="36"/>
       <c r="N31" s="46"/>
-      <c r="Z31" s="36"/>
-      <c r="AD31" s="36"/>
+      <c r="Y31" s="36"/>
+      <c r="AC31" s="36"/>
+      <c r="AH31" s="36"/>
       <c r="AI31" s="36"/>
-      <c r="AJ31" s="36"/>
-      <c r="AS31" s="36"/>
-    </row>
-    <row r="32" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR31" s="36"/>
+    </row>
+    <row r="32" spans="6:44" ht="18.75" customHeight="1">
       <c r="F32" s="46"/>
       <c r="M32" s="36"/>
       <c r="N32" s="46"/>
-      <c r="Z32" s="36"/>
-      <c r="AD32" s="36"/>
+      <c r="Y32" s="36"/>
+      <c r="AC32" s="36"/>
+      <c r="AH32" s="36"/>
       <c r="AI32" s="36"/>
-      <c r="AJ32" s="36"/>
-      <c r="AS32" s="36"/>
-    </row>
-    <row r="33" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR32" s="36"/>
+    </row>
+    <row r="33" spans="6:44" ht="18.75" customHeight="1">
       <c r="F33" s="46"/>
       <c r="M33" s="36"/>
       <c r="N33" s="46"/>
-      <c r="Z33" s="36"/>
-      <c r="AD33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="AC33" s="36"/>
+      <c r="AH33" s="36"/>
       <c r="AI33" s="36"/>
-      <c r="AJ33" s="36"/>
-      <c r="AS33" s="36"/>
-    </row>
-    <row r="34" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR33" s="36"/>
+    </row>
+    <row r="34" spans="6:44" ht="18.75" customHeight="1">
       <c r="F34" s="46"/>
       <c r="M34" s="36"/>
       <c r="N34" s="46"/>
-      <c r="Z34" s="36"/>
-      <c r="AD34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="AC34" s="36"/>
+      <c r="AH34" s="36"/>
       <c r="AI34" s="36"/>
-      <c r="AJ34" s="36"/>
-      <c r="AS34" s="36"/>
-    </row>
-    <row r="35" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR34" s="36"/>
+    </row>
+    <row r="35" spans="6:44" ht="18.75" customHeight="1">
       <c r="F35" s="46"/>
       <c r="M35" s="36"/>
       <c r="N35" s="46"/>
-      <c r="Z35" s="36"/>
-      <c r="AD35" s="36"/>
+      <c r="Y35" s="36"/>
+      <c r="AC35" s="36"/>
+      <c r="AH35" s="36"/>
       <c r="AI35" s="36"/>
-      <c r="AJ35" s="36"/>
-      <c r="AS35" s="36"/>
-    </row>
-    <row r="36" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR35" s="36"/>
+    </row>
+    <row r="36" spans="6:44" ht="18.75" customHeight="1">
       <c r="F36" s="46"/>
       <c r="M36" s="36"/>
       <c r="N36" s="46"/>
-      <c r="Z36" s="36"/>
-      <c r="AD36" s="36"/>
+      <c r="Y36" s="36"/>
+      <c r="AC36" s="36"/>
+      <c r="AH36" s="36"/>
       <c r="AI36" s="36"/>
-      <c r="AJ36" s="36"/>
-      <c r="AS36" s="36"/>
-    </row>
-    <row r="37" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR36" s="36"/>
+    </row>
+    <row r="37" spans="6:44" ht="18.75" customHeight="1">
       <c r="F37" s="46"/>
       <c r="M37" s="36"/>
       <c r="N37" s="46"/>
-      <c r="Z37" s="36"/>
-      <c r="AD37" s="36"/>
+      <c r="Y37" s="36"/>
+      <c r="AC37" s="36"/>
+      <c r="AH37" s="36"/>
       <c r="AI37" s="36"/>
-      <c r="AJ37" s="36"/>
-      <c r="AS37" s="36"/>
-    </row>
-    <row r="38" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR37" s="36"/>
+    </row>
+    <row r="38" spans="6:44" ht="18.75" customHeight="1">
       <c r="F38" s="46"/>
       <c r="M38" s="36"/>
       <c r="N38" s="46"/>
-      <c r="Z38" s="36"/>
-      <c r="AD38" s="36"/>
+      <c r="Y38" s="36"/>
+      <c r="AC38" s="36"/>
+      <c r="AH38" s="36"/>
       <c r="AI38" s="36"/>
-      <c r="AJ38" s="36"/>
-      <c r="AS38" s="36"/>
-    </row>
-    <row r="39" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR38" s="36"/>
+    </row>
+    <row r="39" spans="6:44" ht="18.75" customHeight="1">
       <c r="F39" s="46"/>
       <c r="M39" s="36"/>
       <c r="N39" s="46"/>
-      <c r="Z39" s="36"/>
-      <c r="AD39" s="36"/>
+      <c r="Y39" s="36"/>
+      <c r="AC39" s="36"/>
+      <c r="AH39" s="36"/>
       <c r="AI39" s="36"/>
-      <c r="AJ39" s="36"/>
-      <c r="AS39" s="36"/>
-    </row>
-    <row r="40" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR39" s="36"/>
+    </row>
+    <row r="40" spans="6:44" ht="18.75" customHeight="1">
       <c r="F40" s="46"/>
       <c r="M40" s="36"/>
       <c r="N40" s="46"/>
-      <c r="Z40" s="36"/>
-      <c r="AD40" s="36"/>
+      <c r="Y40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AH40" s="36"/>
       <c r="AI40" s="36"/>
-      <c r="AJ40" s="36"/>
-      <c r="AS40" s="36"/>
-    </row>
-    <row r="41" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR40" s="36"/>
+    </row>
+    <row r="41" spans="6:44" ht="18.75" customHeight="1">
       <c r="F41" s="46"/>
       <c r="M41" s="36"/>
       <c r="N41" s="46"/>
-      <c r="Z41" s="36"/>
-      <c r="AD41" s="36"/>
+      <c r="Y41" s="36"/>
+      <c r="AC41" s="36"/>
+      <c r="AH41" s="36"/>
       <c r="AI41" s="36"/>
-      <c r="AJ41" s="36"/>
-      <c r="AS41" s="36"/>
-    </row>
-    <row r="42" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR41" s="36"/>
+    </row>
+    <row r="42" spans="6:44" ht="18.75" customHeight="1">
       <c r="F42" s="46"/>
       <c r="M42" s="36"/>
       <c r="N42" s="46"/>
-      <c r="Z42" s="36"/>
-      <c r="AD42" s="36"/>
+      <c r="Y42" s="36"/>
+      <c r="AC42" s="36"/>
+      <c r="AH42" s="36"/>
       <c r="AI42" s="36"/>
-      <c r="AJ42" s="36"/>
-      <c r="AS42" s="36"/>
-    </row>
-    <row r="43" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR42" s="36"/>
+    </row>
+    <row r="43" spans="6:44" ht="18.75" customHeight="1">
       <c r="F43" s="46"/>
       <c r="M43" s="36"/>
       <c r="N43" s="46"/>
-      <c r="Z43" s="36"/>
-      <c r="AD43" s="36"/>
+      <c r="Y43" s="36"/>
+      <c r="AC43" s="36"/>
+      <c r="AH43" s="36"/>
       <c r="AI43" s="36"/>
-      <c r="AJ43" s="36"/>
-      <c r="AS43" s="36"/>
-    </row>
-    <row r="44" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR43" s="36"/>
+    </row>
+    <row r="44" spans="6:44" ht="18.75" customHeight="1">
       <c r="F44" s="46"/>
       <c r="M44" s="36"/>
       <c r="N44" s="46"/>
-      <c r="Z44" s="36"/>
-      <c r="AD44" s="36"/>
+      <c r="Y44" s="36"/>
+      <c r="AC44" s="36"/>
+      <c r="AH44" s="36"/>
       <c r="AI44" s="36"/>
-      <c r="AJ44" s="36"/>
-      <c r="AS44" s="36"/>
-    </row>
-    <row r="45" spans="6:45" ht="18.75" customHeight="1">
+      <c r="AR44" s="36"/>
+    </row>
+    <row r="45" spans="6:44" ht="18.75" customHeight="1">
       <c r="F45" s="46"/>
       <c r="M45" s="36"/>
       <c r="N45" s="46"/>
-      <c r="Z45" s="36"/>
-      <c r="AD45" s="36"/>
+      <c r="Y45" s="36"/>
+      <c r="AC45" s="36"/>
+      <c r="AH45" s="36"/>
       <c r="AI45" s="36"/>
-      <c r="AJ45" s="36"/>
-      <c r="AS45" s="36"/>
+      <c r="AR45" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6854,6 +6890,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -6862,61 +6953,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>